<commit_message>
validate excel before importing employees, default password is 123456
</commit_message>
<xml_diff>
--- a/employee-evaluation/src/main/resources/templates/employee_import_template.xlsx
+++ b/employee-evaluation/src/main/resources/templates/employee_import_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CODING\code\java\intern\employee-evaluation\src\main\resources\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{322B71CA-A795-4585-8896-C6FC0399D890}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A601282C-40C1-48AB-AF7E-202861C3BDE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Mã nhân viên</t>
   </si>
@@ -101,6 +101,9 @@
   </si>
   <si>
     <t>JUNIOR</t>
+  </si>
+  <si>
+    <t>Username</t>
   </si>
 </sst>
 </file>
@@ -446,10 +449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -460,9 +463,10 @@
     <col min="4" max="4" width="25.7109375" customWidth="1"/>
     <col min="5" max="5" width="24.85546875" customWidth="1"/>
     <col min="6" max="6" width="31.85546875" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -481,10 +485,13 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="G1" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>